<commit_message>
Small changes to run example as suggested by Spalding
</commit_message>
<xml_diff>
--- a/xls2xml/tests/data/example_EGA_submission.V5.xlsx
+++ b/xls2xml/tests/data/example_EGA_submission.V5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zl/work/ega-submissions/xls2xml/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD4DE3B-646B-9848-A5F8-3E62E7ADFAC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A2A056-1579-254B-B6FB-E44C796828B2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38360" windowHeight="21140" firstSheet="1" activeTab="17" xr2:uid="{B97D998F-FDD8-5440-ACAC-8270B7EF3683}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38360" windowHeight="21140" firstSheet="7" activeTab="10" xr2:uid="{B97D998F-FDD8-5440-ACAC-8270B7EF3683}"/>
   </bookViews>
   <sheets>
     <sheet name="Please Read First" sheetId="26" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="653">
   <si>
     <t>Column Header</t>
   </si>
@@ -1993,9 +1993,6 @@
     <t>van_RoonMom</t>
   </si>
   <si>
-    <t>HDRNAseq</t>
-  </si>
-  <si>
     <t>HD</t>
   </si>
   <si>
@@ -2023,9 +2020,6 @@
     <t>Cologne</t>
   </si>
   <si>
-    <t>SMA_LMND_WGS</t>
-  </si>
-  <si>
     <t>SMA_LMND</t>
   </si>
   <si>
@@ -2132,9 +2126,6 @@
   </si>
   <si>
     <t>Characteristic - deCODE_Rseq_barcode</t>
-  </si>
-  <si>
-    <t>HDRseq</t>
   </si>
   <si>
     <t>Unique id for the experiment (From Experiment sheet). Comma separated list allowable for multiple experiments.</t>
@@ -2557,11 +2548,11 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
@@ -2921,7 +2912,7 @@
       <c r="B1" s="52"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="53" t="s">
         <v>52</v>
       </c>
       <c r="B2" s="52"/>
@@ -2965,10 +2956,10 @@
       <c r="B10" s="52"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="54" t="s">
         <v>507</v>
       </c>
-      <c r="B11" s="54"/>
+      <c r="B11" s="55"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="9" t="s">
@@ -3076,12 +3067,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
@@ -3091,6 +3076,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3345,15 +3336,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C9F7AD-01A4-7F4E-ACB0-C927A3B5A11E}">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="5" width="29.5" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" customWidth="1"/>
@@ -3480,13 +3471,13 @@
     <row r="2" spans="1:23">
       <c r="A2" s="7"/>
       <c r="B2" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="C2" t="s">
-        <v>585</v>
+        <v>632</v>
       </c>
       <c r="D2" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="G2" t="s">
         <v>250</v>
@@ -3501,13 +3492,13 @@
         <v>300</v>
       </c>
       <c r="M2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="S2" t="s">
         <v>432</v>
       </c>
       <c r="T2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="V2" t="s">
         <v>545</v>
@@ -3515,13 +3506,13 @@
     </row>
     <row r="3" spans="1:23">
       <c r="B3" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C3" t="s">
-        <v>595</v>
+        <v>633</v>
       </c>
       <c r="D3" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -3545,21 +3536,21 @@
         <v>432</v>
       </c>
       <c r="T3" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="V3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="B4" t="s">
+        <v>634</v>
+      </c>
+      <c r="C4" t="s">
+        <v>634</v>
+      </c>
+      <c r="D4" t="s">
         <v>637</v>
-      </c>
-      <c r="C4" t="s">
-        <v>595</v>
-      </c>
-      <c r="D4" t="s">
-        <v>640</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -3583,21 +3574,21 @@
         <v>432</v>
       </c>
       <c r="T4" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="V4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="B5" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C5" t="s">
-        <v>595</v>
+        <v>635</v>
       </c>
       <c r="D5" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -3621,10 +3612,10 @@
         <v>432</v>
       </c>
       <c r="T5" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="V5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -4520,7 +4511,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4583,13 +4574,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="B2" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C2" t="s">
-        <v>585</v>
+        <v>638</v>
       </c>
       <c r="D2" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="H2" t="s">
         <v>545</v>
@@ -4597,44 +4588,44 @@
     </row>
     <row r="3" spans="1:8">
       <c r="B3" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C3" t="s">
-        <v>595</v>
+        <v>639</v>
       </c>
       <c r="D3" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="H3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="B4" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="C4" t="s">
-        <v>595</v>
+        <v>640</v>
       </c>
       <c r="D4" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="B5" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C5" t="s">
-        <v>595</v>
+        <v>641</v>
       </c>
       <c r="D5" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="H5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
   </sheetData>
@@ -4736,7 +4727,7 @@
         <v>418</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4765,7 +4756,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="39" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B13" s="5"/>
     </row>
@@ -4781,7 +4772,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="5" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>557</v>
@@ -4842,7 +4833,7 @@
   <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4916,7 +4907,7 @@
         <v>79</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="M1" s="39" t="s">
         <v>550</v>
@@ -4925,78 +4916,78 @@
         <v>553</v>
       </c>
       <c r="O1" s="39" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="P1" s="36" t="s">
+        <v>611</v>
+      </c>
+      <c r="Q1" s="36" t="s">
+        <v>629</v>
+      </c>
+      <c r="R1" s="36" t="s">
+        <v>612</v>
+      </c>
+      <c r="S1" s="38" t="s">
         <v>613</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="T1" s="36" t="s">
+        <v>614</v>
+      </c>
+      <c r="U1" s="38" t="s">
+        <v>615</v>
+      </c>
+      <c r="V1" s="38" t="s">
+        <v>616</v>
+      </c>
+      <c r="W1" s="38" t="s">
         <v>631</v>
       </c>
-      <c r="R1" s="36" t="s">
-        <v>614</v>
-      </c>
-      <c r="S1" s="38" t="s">
-        <v>615</v>
-      </c>
-      <c r="T1" s="36" t="s">
-        <v>616</v>
-      </c>
-      <c r="U1" s="38" t="s">
+      <c r="X1" s="38" t="s">
         <v>617</v>
       </c>
-      <c r="V1" s="38" t="s">
+      <c r="Y1" s="38" t="s">
         <v>618</v>
       </c>
-      <c r="W1" s="38" t="s">
-        <v>634</v>
-      </c>
-      <c r="X1" s="38" t="s">
+      <c r="Z1" s="38" t="s">
         <v>619</v>
       </c>
-      <c r="Y1" s="38" t="s">
+      <c r="AA1" s="38" t="s">
         <v>620</v>
       </c>
-      <c r="Z1" s="38" t="s">
+      <c r="AB1" s="38" t="s">
         <v>621</v>
       </c>
-      <c r="AA1" s="38" t="s">
+      <c r="AC1" s="38" t="s">
         <v>622</v>
       </c>
-      <c r="AB1" s="38" t="s">
+      <c r="AD1" s="38" t="s">
         <v>623</v>
       </c>
-      <c r="AC1" s="38" t="s">
+      <c r="AE1" s="38" t="s">
         <v>624</v>
       </c>
-      <c r="AD1" s="38" t="s">
+      <c r="AF1" s="38" t="s">
         <v>625</v>
       </c>
-      <c r="AE1" s="38" t="s">
+      <c r="AG1" s="38" t="s">
         <v>626</v>
       </c>
-      <c r="AF1" s="38" t="s">
+      <c r="AH1" s="38" t="s">
         <v>627</v>
-      </c>
-      <c r="AG1" s="38" t="s">
-        <v>628</v>
-      </c>
-      <c r="AH1" s="38" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="2" spans="1:34">
       <c r="B2" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C2" t="s">
-        <v>632</v>
+        <v>642</v>
       </c>
       <c r="F2" t="s">
         <v>545</v>
       </c>
       <c r="H2" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="L2">
         <v>9606</v>
@@ -5005,7 +4996,7 @@
         <v>552</v>
       </c>
       <c r="N2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="S2" t="s">
         <v>556</v>
@@ -5014,21 +5005,21 @@
         <v>584</v>
       </c>
       <c r="U2" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="3" spans="1:34">
       <c r="B3" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="C3" t="s">
-        <v>595</v>
+        <v>643</v>
       </c>
       <c r="F3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H3" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="L3">
         <v>9606</v>
@@ -5040,39 +5031,39 @@
         <v>554</v>
       </c>
       <c r="P3" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="S3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="T3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="U3" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="Y3" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="AG3" t="s">
         <v>555</v>
       </c>
       <c r="AH3" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="4" spans="1:34">
       <c r="B4" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C4" t="s">
-        <v>595</v>
+        <v>644</v>
       </c>
       <c r="F4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H4" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="L4">
         <v>9606</v>
@@ -5084,39 +5075,39 @@
         <v>554</v>
       </c>
       <c r="P4" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="S4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="T4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="U4" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="Y4" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="AG4" t="s">
         <v>555</v>
       </c>
       <c r="AH4" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="5" spans="1:34">
       <c r="B5" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="C5" t="s">
-        <v>595</v>
+        <v>645</v>
       </c>
       <c r="F5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H5" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="L5">
         <v>9606</v>
@@ -5125,37 +5116,37 @@
         <v>551</v>
       </c>
       <c r="N5" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="P5" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="R5" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="S5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="T5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="U5" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="V5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="W5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="X5" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="AG5" t="s">
         <v>555</v>
       </c>
       <c r="AH5" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
   </sheetData>
@@ -5283,7 +5274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85792D68-D418-C748-8F64-73FBA35DD965}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -5322,117 +5313,117 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G2" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G3" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D4" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E4" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F4" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G4" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E5" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="F5" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G5" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D6" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="E6" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F6" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G6" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix titles in the test data examples for Run, Experiment and Sample
</commit_message>
<xml_diff>
--- a/xls2xml/tests/data/example_EGA_submission.V5.xlsx
+++ b/xls2xml/tests/data/example_EGA_submission.V5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zl/work/ega-submissions/xls2xml/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A2A056-1579-254B-B6FB-E44C796828B2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBBC129-8660-C848-B246-7312EE30B052}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38360" windowHeight="21140" firstSheet="7" activeTab="10" xr2:uid="{B97D998F-FDD8-5440-ACAC-8270B7EF3683}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38360" windowHeight="21140" activeTab="17" xr2:uid="{B97D998F-FDD8-5440-ACAC-8270B7EF3683}"/>
   </bookViews>
   <sheets>
     <sheet name="Please Read First" sheetId="26" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="665">
   <si>
     <t>Column Header</t>
   </si>
@@ -2195,6 +2195,42 @@
   </si>
   <si>
     <t>BAMs/Samp004.bam.gpg</t>
+  </si>
+  <si>
+    <t>HDRNAseq Exp001</t>
+  </si>
+  <si>
+    <t>SMA_LMND_WGS Exp002</t>
+  </si>
+  <si>
+    <t>SMA_LMND_WGS Exp003</t>
+  </si>
+  <si>
+    <t>SMA_LMND_WGS Exp004</t>
+  </si>
+  <si>
+    <t>HDRNAseq Run001</t>
+  </si>
+  <si>
+    <t>SMA_LMND_WGS Run002</t>
+  </si>
+  <si>
+    <t>SMA_LMND_WGS Run003</t>
+  </si>
+  <si>
+    <t>SMA_LMND_WGS Run004</t>
+  </si>
+  <si>
+    <t>HDRseq Samp001</t>
+  </si>
+  <si>
+    <t>SMA_LMND_WGS Samp002</t>
+  </si>
+  <si>
+    <t>SMA_LMND_WGS Samp003</t>
+  </si>
+  <si>
+    <t>SMA_LMND_WGS Samp004</t>
   </si>
 </sst>
 </file>
@@ -3336,15 +3372,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C9F7AD-01A4-7F4E-ACB0-C927A3B5A11E}">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.5" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="5" width="29.5" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" customWidth="1"/>
@@ -3474,7 +3510,7 @@
         <v>632</v>
       </c>
       <c r="C2" t="s">
-        <v>632</v>
+        <v>653</v>
       </c>
       <c r="D2" t="s">
         <v>636</v>
@@ -3509,7 +3545,7 @@
         <v>633</v>
       </c>
       <c r="C3" t="s">
-        <v>633</v>
+        <v>654</v>
       </c>
       <c r="D3" t="s">
         <v>637</v>
@@ -3547,7 +3583,7 @@
         <v>634</v>
       </c>
       <c r="C4" t="s">
-        <v>634</v>
+        <v>655</v>
       </c>
       <c r="D4" t="s">
         <v>637</v>
@@ -3585,7 +3621,7 @@
         <v>635</v>
       </c>
       <c r="C5" t="s">
-        <v>635</v>
+        <v>656</v>
       </c>
       <c r="D5" t="s">
         <v>637</v>
@@ -4511,12 +4547,12 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" customWidth="1"/>
@@ -4577,7 +4613,7 @@
         <v>638</v>
       </c>
       <c r="C2" t="s">
-        <v>638</v>
+        <v>657</v>
       </c>
       <c r="D2" t="s">
         <v>632</v>
@@ -4591,7 +4627,7 @@
         <v>639</v>
       </c>
       <c r="C3" t="s">
-        <v>639</v>
+        <v>658</v>
       </c>
       <c r="D3" t="s">
         <v>633</v>
@@ -4605,7 +4641,7 @@
         <v>640</v>
       </c>
       <c r="C4" t="s">
-        <v>640</v>
+        <v>659</v>
       </c>
       <c r="D4" t="s">
         <v>634</v>
@@ -4619,7 +4655,7 @@
         <v>641</v>
       </c>
       <c r="C5" t="s">
-        <v>641</v>
+        <v>660</v>
       </c>
       <c r="D5" t="s">
         <v>635</v>
@@ -4833,7 +4869,7 @@
   <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4981,7 +5017,7 @@
         <v>642</v>
       </c>
       <c r="C2" t="s">
-        <v>642</v>
+        <v>661</v>
       </c>
       <c r="F2" t="s">
         <v>545</v>
@@ -5013,7 +5049,7 @@
         <v>643</v>
       </c>
       <c r="C3" t="s">
-        <v>643</v>
+        <v>662</v>
       </c>
       <c r="F3" t="s">
         <v>591</v>
@@ -5057,7 +5093,7 @@
         <v>644</v>
       </c>
       <c r="C4" t="s">
-        <v>644</v>
+        <v>663</v>
       </c>
       <c r="F4" t="s">
         <v>591</v>
@@ -5101,7 +5137,7 @@
         <v>645</v>
       </c>
       <c r="C5" t="s">
-        <v>645</v>
+        <v>664</v>
       </c>
       <c r="F5" t="s">
         <v>591</v>
@@ -5274,7 +5310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85792D68-D418-C748-8F64-73FBA35DD965}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>